<commit_message>
files: updation plus addition
</commit_message>
<xml_diff>
--- a/Sarepta Therapeutics/Models/FCFF take0.xlsx
+++ b/Sarepta Therapeutics/Models/FCFF take0.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Financial-Models\Sarepta Therapeutics\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F51C9C-A4BF-4383-887A-0ED0B16E1893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D47F107-B075-480E-AB85-0D1FC92BCB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{97F628CD-3962-40D6-8CC6-06D54CDF64AE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Historical Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Basic Assumptions" sheetId="2" r:id="rId1"/>
+    <sheet name="Historical Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Sarepta Therapeutics</t>
   </si>
@@ -109,6 +110,15 @@
   </si>
   <si>
     <t>Operating Loss</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Risk free rate</t>
   </si>
 </sst>
 </file>
@@ -117,7 +127,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="169" formatCode="#,##0;\(#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="#,##0;\(#,##0\)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -190,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -205,19 +215,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -226,6 +230,13 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -540,11 +551,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069CF035-493D-4003-88E0-8488EC920214}">
+  <dimension ref="A3:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="13">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9840831-88D1-4BE1-8006-508D3D2F1F22}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,21 +606,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D3" s="2" t="s">
@@ -649,47 +695,47 @@
         <v>1901979</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <f>(D4-C4)/C4</f>
         <v>-0.87157937890745107</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="10">
         <f t="shared" ref="E5:M5" si="0">(E4-D4)/D4</f>
         <v>3.3264166001596167</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <f t="shared" si="0"/>
         <v>27.515771997786388</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="10">
         <f t="shared" si="0"/>
         <v>0.94738135900222531</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="10">
         <f t="shared" si="0"/>
         <v>0.26508301387883099</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="10">
         <f t="shared" si="0"/>
         <v>0.41820430477400855</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="10">
         <f t="shared" si="0"/>
         <v>0.29955248945100804</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="10">
         <f t="shared" si="0"/>
         <v>0.32929232198345315</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="10">
         <f t="shared" si="0"/>
         <v>0.33260308270088412</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="10">
         <f t="shared" si="0"/>
         <v>0.52973854211572735</v>
       </c>
@@ -727,12 +773,18 @@
       <c r="K8" s="1">
         <v>139989</v>
       </c>
+      <c r="L8" s="1">
+        <v>150343</v>
+      </c>
+      <c r="M8" s="1">
+        <v>319099</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="6">
         <v>188272</v>
       </c>
       <c r="F9" s="1">
@@ -752,6 +804,12 @@
       </c>
       <c r="K9" s="1">
         <v>877090</v>
+      </c>
+      <c r="L9" s="1">
+        <v>877387</v>
+      </c>
+      <c r="M9" s="1">
+        <v>804522</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -779,18 +837,24 @@
       <c r="K10" s="1">
         <v>451421</v>
       </c>
+      <c r="L10" s="1">
+        <v>481871</v>
+      </c>
+      <c r="M10" s="1">
+        <v>557872</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="8" t="s">
+      <c r="E11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="1">
@@ -803,6 +867,12 @@
         <v>19</v>
       </c>
       <c r="K11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -810,13 +880,13 @@
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="1">
         <v>28427</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="H12" s="1">
@@ -829,6 +899,12 @@
         <v>10000</v>
       </c>
       <c r="K12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -836,7 +912,7 @@
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="1">
@@ -856,72 +932,94 @@
       </c>
       <c r="K13">
         <v>714</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1559</v>
+      </c>
+      <c r="M13" s="1">
+        <v>2405</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <f>SUM(E8:E13)</f>
         <v>272151</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <f t="shared" ref="F14:H14" si="1">SUM(F8:F13)</f>
         <v>326222</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="7">
         <f t="shared" si="1"/>
         <v>644662</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="7">
         <f t="shared" si="1"/>
         <v>1086396</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="7">
         <f t="shared" ref="I14" si="2">SUM(I8:I13)</f>
         <v>1104262</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="7">
         <f t="shared" ref="J14" si="3">SUM(J8:J13)</f>
         <v>1161597</v>
       </c>
-      <c r="K14" s="9">
-        <f t="shared" ref="K14" si="4">SUM(K8:K13)</f>
+      <c r="K14" s="7">
+        <f t="shared" ref="K14:M14" si="4">SUM(K8:K13)</f>
         <v>1469214</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="4"/>
+        <v>1511160</v>
+      </c>
+      <c r="M14" s="7">
+        <f t="shared" si="4"/>
+        <v>1683898</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="8">
         <f>E4-E14</f>
         <v>-266730</v>
       </c>
-      <c r="F16" s="10">
-        <f t="shared" ref="F16:K16" si="5">F4-F14</f>
+      <c r="F16" s="8">
+        <f t="shared" ref="F16:M16" si="5">F4-F14</f>
         <v>-171638</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="8">
         <f t="shared" si="5"/>
         <v>-343628</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="8">
         <f t="shared" si="5"/>
         <v>-705563</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="8">
         <f t="shared" si="5"/>
         <v>-564163</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="8">
         <f t="shared" si="5"/>
         <v>-459710</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="8">
         <f t="shared" si="5"/>
         <v>-536201</v>
+      </c>
+      <c r="L16" s="8">
+        <f t="shared" si="5"/>
+        <v>-267824</v>
+      </c>
+      <c r="M16" s="8">
+        <f t="shared" si="5"/>
+        <v>218081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>